<commit_message>
Template Selection Logic Comleted
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AEFBCE-17C5-42ED-98CF-F35DE8CEF504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4615E4-666B-48E9-8774-607CE3ED79AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -176,9 +176,6 @@
     <t>OfferLetterList</t>
   </si>
   <si>
-    <t>P004_SP002_090_NHC_OLC_Dispatcher_Queue</t>
-  </si>
-  <si>
     <t>DEV</t>
   </si>
   <si>
@@ -197,12 +194,6 @@
     <t>Birth|(Email</t>
   </si>
   <si>
-    <t>NameNewLineException</t>
-  </si>
-  <si>
-    <t>Empty line found in the extracted name from the pdf file.</t>
-  </si>
-  <si>
     <t>Number of characters found in the extracted name is less than 5.</t>
   </si>
   <si>
@@ -308,14 +299,110 @@
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>AddtoQueue</t>
+    <t>P004_SP002_090_NHC_OLC_Performer_Queue</t>
+  </si>
+  <si>
+    <t>OfferLetter_Date</t>
+  </si>
+  <si>
+    <t>OfferLetter_Name</t>
+  </si>
+  <si>
+    <t>OfferLetter_Address</t>
+  </si>
+  <si>
+    <t>OfferLetter_City</t>
+  </si>
+  <si>
+    <t>OfferLetter_State</t>
+  </si>
+  <si>
+    <t>OfferLetter_LastName</t>
+  </si>
+  <si>
+    <t>OfferLetter_Salary</t>
+  </si>
+  <si>
+    <t>OfferLetter_JobTitle</t>
+  </si>
+  <si>
+    <t>__Date__</t>
+  </si>
+  <si>
+    <t>__Name__</t>
+  </si>
+  <si>
+    <t>__LastName__</t>
+  </si>
+  <si>
+    <t>__Address__</t>
+  </si>
+  <si>
+    <t>__City__</t>
+  </si>
+  <si>
+    <t>__State__</t>
+  </si>
+  <si>
+    <t>__JobTitle__</t>
+  </si>
+  <si>
+    <t>__Salary__</t>
+  </si>
+  <si>
+    <t>JRNotFoundException</t>
+  </si>
+  <si>
+    <t>Job Reference Number not found in WorkDay</t>
+  </si>
+  <si>
+    <t>Template_Exempt_With_Trial</t>
+  </si>
+  <si>
+    <t>Template_Exempt_Without_Trial</t>
+  </si>
+  <si>
+    <t>Template_NonExempt_With_Trial</t>
+  </si>
+  <si>
+    <t>Template_NonExempt_Without_Trial</t>
+  </si>
+  <si>
+    <t>Template_Executive</t>
+  </si>
+  <si>
+    <t>Template_Temporary</t>
+  </si>
+  <si>
+    <t>OfferLetterTemplateFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\Input\Templates\</t>
+  </si>
+  <si>
+    <t>Exempt - with Trial Period.docx</t>
+  </si>
+  <si>
+    <t>Exempt - without Trial Period.docx</t>
+  </si>
+  <si>
+    <t>Nonexempt - with Trial Period.docx</t>
+  </si>
+  <si>
+    <t>Nonexempt - without Trial Period.docx</t>
+  </si>
+  <si>
+    <t>X 5%.docx</t>
+  </si>
+  <si>
+    <t>X 999 Temp.docx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -345,6 +432,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -367,7 +460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -381,6 +474,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -696,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -746,10 +840,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -760,7 +854,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -772,7 +866,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -780,35 +874,35 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
         <v>64</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -824,7 +918,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B11" t="s">
@@ -844,118 +938,216 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
-      </c>
-    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A29" t="s">
-        <v>71</v>
+      <c r="A29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>86</v>
+      <c r="A32" t="s">
+        <v>93</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>90</v>
+      <c r="A34" t="s">
+        <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>94</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>96</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A43" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" t="s">
+        <v>123</v>
+      </c>
+    </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1906,11 +2098,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -1927,7 +2114,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3090,7 +3277,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3139,58 +3326,58 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Word Replace and Send Email Complete
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266440E5-80B7-4782-89AE-D072D000E5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316E97A1-C9E2-4224-811D-89AD342EF689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="134">
   <si>
     <t>Name</t>
   </si>
@@ -302,30 +302,6 @@
     <t>P004_SP002_090_NHC_OLC_Performer_Queue</t>
   </si>
   <si>
-    <t>OfferLetter_Date</t>
-  </si>
-  <si>
-    <t>OfferLetter_Name</t>
-  </si>
-  <si>
-    <t>OfferLetter_Address</t>
-  </si>
-  <si>
-    <t>OfferLetter_City</t>
-  </si>
-  <si>
-    <t>OfferLetter_State</t>
-  </si>
-  <si>
-    <t>OfferLetter_LastName</t>
-  </si>
-  <si>
-    <t>OfferLetter_Salary</t>
-  </si>
-  <si>
-    <t>OfferLetter_JobTitle</t>
-  </si>
-  <si>
     <t>__Date__</t>
   </si>
   <si>
@@ -344,9 +320,6 @@
     <t>__State__</t>
   </si>
   <si>
-    <t>__JobTitle__</t>
-  </si>
-  <si>
     <t>__Salary__</t>
   </si>
   <si>
@@ -396,6 +369,63 @@
   </si>
   <si>
     <t>X 999 Temp.docx</t>
+  </si>
+  <si>
+    <t>TemplateNotFoundException</t>
+  </si>
+  <si>
+    <t>Template cloud not be selected based on given data</t>
+  </si>
+  <si>
+    <t>OfferLetterOutputFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\Output\OfferLetters\</t>
+  </si>
+  <si>
+    <t>__Zip__</t>
+  </si>
+  <si>
+    <t>OfferLetterDate</t>
+  </si>
+  <si>
+    <t>OfferLetterName</t>
+  </si>
+  <si>
+    <t>OfferLetterLastName</t>
+  </si>
+  <si>
+    <t>OfferLetterAddress</t>
+  </si>
+  <si>
+    <t>OfferLetterCity</t>
+  </si>
+  <si>
+    <t>OfferLetterState</t>
+  </si>
+  <si>
+    <t>OfferLetterZip</t>
+  </si>
+  <si>
+    <t>OfferLetterJobTitle</t>
+  </si>
+  <si>
+    <t>OfferLetterSalary</t>
+  </si>
+  <si>
+    <t>__Job Title__</t>
+  </si>
+  <si>
+    <t>HRApprovalMailSubject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offer Letter Approval - </t>
+  </si>
+  <si>
+    <t>OfferLetterSignedExtension</t>
+  </si>
+  <si>
+    <t>_Signed.docx</t>
   </si>
 </sst>
 </file>
@@ -790,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -965,10 +995,10 @@
     <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
@@ -987,7 +1017,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" t="s">
+        <v>116</v>
+      </c>
+    </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
@@ -1030,79 +1067,79 @@
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" t="s">
         <v>92</v>
-      </c>
-      <c r="B31" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" t="s">
         <v>93</v>
-      </c>
-      <c r="B32" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B40" t="s">
         <v>118</v>
@@ -1110,63 +1147,91 @@
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B43" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A46" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" t="s">
+        <v>114</v>
+      </c>
+    </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="49" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A49" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A50" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="52" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="56" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="57" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="58" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="59" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="60" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -2098,6 +2163,8 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -3277,13 +3344,13 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Added logic to send email to New Hire
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316E97A1-C9E2-4224-811D-89AD342EF689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58900DF3-C7C6-4AB5-9494-4B3F3207764D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="140">
   <si>
     <t>Name</t>
   </si>
@@ -179,9 +179,6 @@
     <t>DEV</t>
   </si>
   <si>
-    <t>P004_SP002_090_NHC_OLC_Dispatcher</t>
-  </si>
-  <si>
     <t>NameExtractor</t>
   </si>
   <si>
@@ -426,6 +423,27 @@
   </si>
   <si>
     <t>_Signed.docx</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_NHC_OLC_Performer</t>
+  </si>
+  <si>
+    <t>OfferLetterSignedFolderPath</t>
+  </si>
+  <si>
+    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\Output\SignedOffers\</t>
+  </si>
+  <si>
+    <t>OfferLetterMailSubject</t>
+  </si>
+  <si>
+    <t>Offer Letter to New Hire</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_NHC_WD_Performer_Queue</t>
+  </si>
+  <si>
+    <t>WorkDayDispositioningQueue</t>
   </si>
 </sst>
 </file>
@@ -822,16 +840,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="148.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="148.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -870,16 +888,16 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -891,12 +909,12 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -904,35 +922,35 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -969,260 +987,281 @@
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
         <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" t="s">
         <v>99</v>
-      </c>
-      <c r="B19" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
         <v>58</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" t="s">
         <v>115</v>
-      </c>
-      <c r="B22" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
         <v>78</v>
-      </c>
-      <c r="B26" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" t="s">
         <v>117</v>
-      </c>
-      <c r="B40" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1">
       <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
         <v>107</v>
-      </c>
-      <c r="B41" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" t="s">
         <v>130</v>
-      </c>
-      <c r="B49" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
       <c r="A50" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" t="s">
         <v>132</v>
       </c>
-      <c r="B50" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="51" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" t="s">
+        <v>135</v>
+      </c>
+    </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="53" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A53" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53" t="s">
+        <v>137</v>
+      </c>
+    </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A55" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="57" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="58" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2184,12 +2223,12 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2226,7 +2265,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2237,7 +2276,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -2351,7 +2390,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -3347,12 +3386,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="54.26953125" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3393,58 +3432,58 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
         <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
         <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
         <v>74</v>
-      </c>
-      <c r="B5" t="s">
-        <v>75</v>
       </c>
       <c r="C5" t="s">
         <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Commit before final test
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,21 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58900DF3-C7C6-4AB5-9494-4B3F3207764D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD7837B-4D27-4497-B7BC-BD8EA001714A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="140">
   <si>
     <t>Name</t>
   </si>
@@ -161,48 +174,9 @@
     <t>https://officemgmtentserv.sharepoint.com/sites/NewHireCommunication/Lists/New%20Hire%20Communication%20%20Employee%20Details/OfferLetterTestView.aspx</t>
   </si>
   <si>
-    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\Input\OfferLetterInput.xlsx</t>
-  </si>
-  <si>
-    <t>Dummy Data for Sharepoint</t>
-  </si>
-  <si>
-    <t>OfferLetterInputExcel</t>
-  </si>
-  <si>
-    <t>OfferLetterTableName</t>
-  </si>
-  <si>
-    <t>OfferLetterList</t>
-  </si>
-  <si>
     <t>DEV</t>
   </si>
   <si>
-    <t>NameExtractor</t>
-  </si>
-  <si>
-    <t>applicant.|(First)</t>
-  </si>
-  <si>
-    <t>EmailExtractor</t>
-  </si>
-  <si>
-    <t>Birth|(Email</t>
-  </si>
-  <si>
-    <t>Number of characters found in the extracted name is less than 5.</t>
-  </si>
-  <si>
-    <t>NameInvalidException</t>
-  </si>
-  <si>
-    <t>EmailInvalidException</t>
-  </si>
-  <si>
-    <t>Extracted email is empty or not valid</t>
-  </si>
-  <si>
     <t>Office365_AppID</t>
   </si>
   <si>
@@ -227,15 +201,6 @@
     <t>Office 365 Tenant ID to access Office 365 Apps using API</t>
   </si>
   <si>
-    <t>QueueField_PDFPath</t>
-  </si>
-  <si>
-    <t>BotMailID</t>
-  </si>
-  <si>
-    <t>karthick.sivabalasubramaniam.ctr@omes.ok.gov</t>
-  </si>
-  <si>
     <t>P004_SP002_090_BusinessExceptionContacts</t>
   </si>
   <si>
@@ -323,9 +288,6 @@
     <t>JRNotFoundException</t>
   </si>
   <si>
-    <t>Job Reference Number not found in WorkDay</t>
-  </si>
-  <si>
     <t>Template_Exempt_With_Trial</t>
   </si>
   <si>
@@ -371,9 +333,6 @@
     <t>TemplateNotFoundException</t>
   </si>
   <si>
-    <t>Template cloud not be selected based on given data</t>
-  </si>
-  <si>
     <t>OfferLetterOutputFolder</t>
   </si>
   <si>
@@ -444,6 +403,60 @@
   </si>
   <si>
     <t>WorkDayDispositioningQueue</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_OfferLetterDate</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_OfferLetterName</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_OfferLetterLastName</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_OfferLetterAddress</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_OfferLetterCity</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_OfferLetterState</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_OfferLetterZip</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_OfferLetterJobTitle</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_OfferLetterSalary</t>
+  </si>
+  <si>
+    <t>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</t>
+  </si>
+  <si>
+    <t>Offer Letter Fields</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_Template_Exempt_With_Trial</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_Template_Exempt_Without_Trial</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_Template_NonExempt_With_Trial</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_Template_NonExempt_Without_Trial</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_Template_Executive</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_Template_Temporary</t>
   </si>
 </sst>
 </file>
@@ -838,18 +851,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
-    <col min="2" max="2" width="148.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="148.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -888,33 +901,33 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -922,35 +935,35 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -966,302 +979,135 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-    </row>
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
+      <c r="A14" s="7"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
+      <c r="A15" s="7"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>69</v>
-      </c>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" t="s">
-        <v>115</v>
-      </c>
-    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" t="s">
-        <v>88</v>
-      </c>
-    </row>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
-        <v>119</v>
-      </c>
-      <c r="B31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>120</v>
-      </c>
-      <c r="B32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>121</v>
-      </c>
-      <c r="B33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>122</v>
-      </c>
-      <c r="B34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A35" t="s">
-        <v>123</v>
-      </c>
-      <c r="B35" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A36" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>125</v>
-      </c>
-      <c r="B37" t="s">
-        <v>118</v>
-      </c>
-    </row>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A40" t="s">
-        <v>116</v>
-      </c>
-      <c r="B40" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A41" t="s">
-        <v>106</v>
-      </c>
-      <c r="B41" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A42" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A43" t="s">
-        <v>101</v>
-      </c>
-      <c r="B43" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A44" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A45" t="s">
-        <v>103</v>
-      </c>
-      <c r="B45" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A46" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" t="s">
-        <v>112</v>
-      </c>
-    </row>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:2" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A48" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
+      <c r="B48" t="s">
+        <v>114</v>
+      </c>
+    </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A50" t="s">
-        <v>131</v>
-      </c>
-      <c r="B50" t="s">
-        <v>132</v>
-      </c>
-    </row>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="53" spans="1:2" ht="14.25" customHeight="1">
       <c r="A53" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A55" t="s">
-        <v>139</v>
-      </c>
-      <c r="B55" t="s">
-        <v>138</v>
-      </c>
-    </row>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="56" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="57" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="58" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2202,16 +2048,13 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{3304E173-E629-4825-B4FA-E24275122099}"/>
-    <hyperlink ref="B17" r:id="rId2" xr:uid="{4B3BD2DF-4452-4B7F-BA54-B494AA98EB4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2223,12 +2066,12 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2265,7 +2108,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2276,7 +2119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -2390,7 +2233,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -3383,15 +3226,15 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="54.26953125" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3432,87 +3275,361 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="14.25" customHeight="1">
+      <c r="F26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="str">
+        <f>_xlfn.CONCAT(F27,A27)</f>
+        <v>P004_SP002_090_JRNotFoundException</v>
+      </c>
+      <c r="F27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" t="str">
+        <f>_xlfn.CONCAT(F28,A28)</f>
+        <v>P004_SP002_090_TemplateNotFoundException</v>
+      </c>
+      <c r="F28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="14.25" customHeight="1">
+      <c r="F29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="14.25" customHeight="1">
+      <c r="F30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updates to External Transfer Type
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://officemgmtentserv-my.sharepoint.com/personal/karthick_sivabalasubramaniam_ctr_omes_ok_gov/Documents/Documents/UiPath/P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{5BD7837B-4D27-4497-B7BC-BD8EA001714A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CA6A4FE-2B8A-4534-9548-0DF8F5D34E89}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{5BD7837B-4D27-4497-B7BC-BD8EA001714A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14DC52B7-3018-4B71-9A6A-BC8F8EB0DFC2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="207">
   <si>
     <t>Name</t>
   </si>
@@ -607,6 +607,57 @@
   </si>
   <si>
     <t>SharepointGeneratedFolder</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_PersonNotFound</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_PersonCandidate</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_PersonEmployee</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SummaryTabNotFound</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointSiteURL</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointListFilter</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointList</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointListColumns</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointBGVFolder</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointTemplateFolder</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointGeneratedFolder</t>
+  </si>
+  <si>
+    <t>SharepointSignedFolder</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointSignedFolder</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_HRApprovalMailBody</t>
+  </si>
+  <si>
+    <t>HRApprovalMailBody</t>
+  </si>
+  <si>
+    <t>HRDirectorContact</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_HRDirectorContact</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -4100,9 +4151,8 @@
       <c r="A44" t="s">
         <v>179</v>
       </c>
-      <c r="B44" t="str">
-        <f>_xlfn.CONCAT("P004_SP002_090_",A44)</f>
-        <v>P004_SP002_090_PersonNotFound</v>
+      <c r="B44" t="s">
+        <v>190</v>
       </c>
       <c r="C44" t="s">
         <v>122</v>
@@ -4112,9 +4162,8 @@
       <c r="A45" t="s">
         <v>180</v>
       </c>
-      <c r="B45" t="str">
-        <f t="shared" ref="B45:B55" si="0">_xlfn.CONCAT("P004_SP002_090_",A45)</f>
-        <v>P004_SP002_090_PersonCandidate</v>
+      <c r="B45" t="s">
+        <v>191</v>
       </c>
       <c r="C45" t="s">
         <v>122</v>
@@ -4124,9 +4173,8 @@
       <c r="A46" t="s">
         <v>181</v>
       </c>
-      <c r="B46" t="str">
-        <f t="shared" si="0"/>
-        <v>P004_SP002_090_PersonEmployee</v>
+      <c r="B46" t="s">
+        <v>192</v>
       </c>
       <c r="C46" t="s">
         <v>122</v>
@@ -4136,9 +4184,8 @@
       <c r="A47" t="s">
         <v>182</v>
       </c>
-      <c r="B47" t="str">
-        <f t="shared" si="0"/>
-        <v>P004_SP002_090_SummaryTabNotFound</v>
+      <c r="B47" t="s">
+        <v>193</v>
       </c>
       <c r="C47" t="s">
         <v>122</v>
@@ -4148,9 +4195,8 @@
       <c r="A48" t="s">
         <v>183</v>
       </c>
-      <c r="B48" t="str">
-        <f t="shared" si="0"/>
-        <v>P004_SP002_090_SharepointSiteURL</v>
+      <c r="B48" t="s">
+        <v>194</v>
       </c>
       <c r="C48" t="s">
         <v>122</v>
@@ -4160,9 +4206,8 @@
       <c r="A49" t="s">
         <v>184</v>
       </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>P004_SP002_090_SharepointListFilter</v>
+      <c r="B49" t="s">
+        <v>195</v>
       </c>
       <c r="C49" t="s">
         <v>122</v>
@@ -4172,9 +4217,8 @@
       <c r="A50" t="s">
         <v>185</v>
       </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>P004_SP002_090_SharepointList</v>
+      <c r="B50" t="s">
+        <v>196</v>
       </c>
       <c r="C50" t="s">
         <v>122</v>
@@ -4184,9 +4228,8 @@
       <c r="A51" t="s">
         <v>186</v>
       </c>
-      <c r="B51" t="str">
-        <f t="shared" si="0"/>
-        <v>P004_SP002_090_SharepointListColumns</v>
+      <c r="B51" t="s">
+        <v>197</v>
       </c>
       <c r="C51" t="s">
         <v>122</v>
@@ -4196,9 +4239,8 @@
       <c r="A52" t="s">
         <v>187</v>
       </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>P004_SP002_090_SharepointBGVFolder</v>
+      <c r="B52" t="s">
+        <v>198</v>
       </c>
       <c r="C52" t="s">
         <v>122</v>
@@ -4208,9 +4250,8 @@
       <c r="A53" t="s">
         <v>187</v>
       </c>
-      <c r="B53" t="str">
-        <f t="shared" si="0"/>
-        <v>P004_SP002_090_SharepointBGVFolder</v>
+      <c r="B53" t="s">
+        <v>198</v>
       </c>
       <c r="C53" t="s">
         <v>122</v>
@@ -4220,9 +4261,8 @@
       <c r="A54" t="s">
         <v>188</v>
       </c>
-      <c r="B54" t="str">
-        <f t="shared" si="0"/>
-        <v>P004_SP002_090_SharepointTemplateFolder</v>
+      <c r="B54" t="s">
+        <v>199</v>
       </c>
       <c r="C54" t="s">
         <v>122</v>
@@ -4232,17 +4272,46 @@
       <c r="A55" t="s">
         <v>189</v>
       </c>
-      <c r="B55" t="str">
-        <f t="shared" si="0"/>
-        <v>P004_SP002_090_SharepointGeneratedFolder</v>
+      <c r="B55" t="s">
+        <v>200</v>
       </c>
       <c r="C55" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="56" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A56" t="s">
+        <v>201</v>
+      </c>
+      <c r="B56" t="s">
+        <v>202</v>
+      </c>
+      <c r="C56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A57" t="s">
+        <v>204</v>
+      </c>
+      <c r="B57" t="s">
+        <v>203</v>
+      </c>
+      <c r="C57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A58" t="s">
+        <v>205</v>
+      </c>
+      <c r="B58" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" t="s">
+        <v>122</v>
+      </c>
+    </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="61" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Implemented new changes and updated code after code review.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://officemgmtentserv-my.sharepoint.com/personal/karthick_sivabalasubramaniam_ctr_omes_ok_gov/Documents/Documents/UiPath/P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\OneDrive - State of Oklahoma\Desktop\NHC_OLC_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="13_ncr:1_{5BD7837B-4D27-4497-B7BC-BD8EA001714A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E52E70FA-934C-48AC-A2EF-8682DC493E6C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA24FC3A-7306-4E0D-A6B4-8F1F1CF4903A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="236">
   <si>
     <t>Name</t>
   </si>
@@ -165,15 +165,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>SharePointURL</t>
-  </si>
-  <si>
-    <t>URL of SharepointData Input</t>
-  </si>
-  <si>
-    <t>https://officemgmtentserv.sharepoint.com/sites/NewHireCommunication/Lists/New%20Hire%20Communication%20%20Employee%20Details/OfferLetterTestView.aspx</t>
-  </si>
-  <si>
     <t>DEV</t>
   </si>
   <si>
@@ -285,12 +276,6 @@
     <t>Template_Temporary</t>
   </si>
   <si>
-    <t>OfferLetterTemplateFolder</t>
-  </si>
-  <si>
-    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\Input\Templates\</t>
-  </si>
-  <si>
     <t>Exempt - with Trial Period.docx</t>
   </si>
   <si>
@@ -312,12 +297,6 @@
     <t>TemplateNotFoundException</t>
   </si>
   <si>
-    <t>OfferLetterOutputFolder</t>
-  </si>
-  <si>
-    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\Output\OfferLetters\</t>
-  </si>
-  <si>
     <t>__Zip__</t>
   </si>
   <si>
@@ -357,18 +336,9 @@
     <t>OfferLetterSignedExtension</t>
   </si>
   <si>
-    <t>_Signed.docx</t>
-  </si>
-  <si>
     <t>P004_SP002_090_NHC_OLC_Performer</t>
   </si>
   <si>
-    <t>OfferLetterSignedFolderPath</t>
-  </si>
-  <si>
-    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\Output\SignedOffers\</t>
-  </si>
-  <si>
     <t>OfferLetterMailSubject</t>
   </si>
   <si>
@@ -718,13 +688,70 @@
   </si>
   <si>
     <t>P004_SP002_090_ContactTabNotFound</t>
+  </si>
+  <si>
+    <t>FileDownloadDelay</t>
+  </si>
+  <si>
+    <t>00:01:00</t>
+  </si>
+  <si>
+    <t>This is a string format delay 00:01:00 format</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_OfferLetterSignedExtension</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SignedOfferletterDataNotMatch</t>
+  </si>
+  <si>
+    <t>SignedOfferletterDataNotMatch</t>
+  </si>
+  <si>
+    <t>DaysToAddForMonday</t>
+  </si>
+  <si>
+    <t>DaysToAddForTuesday</t>
+  </si>
+  <si>
+    <t>DaysToAddForWednesday</t>
+  </si>
+  <si>
+    <t>DaysToAddForThrusday</t>
+  </si>
+  <si>
+    <t>DaysToAddForFriday</t>
+  </si>
+  <si>
+    <t>ServiceDateNotValid</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_ServiceDateNotValid</t>
+  </si>
+  <si>
+    <t>ForEmployeeSignedEmailCcContacts</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_ForEmployeeSignedEmailCcContacts</t>
+  </si>
+  <si>
+    <t>HrEmailContactsCC</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_HrEmailContactsCC</t>
+  </si>
+  <si>
+    <t>ProcessToKill</t>
+  </si>
+  <si>
+    <t>msedge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -748,18 +775,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -778,11 +793,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -792,14 +806,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -815,14 +824,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -860,7 +865,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -966,7 +971,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1108,7 +1113,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1116,18 +1121,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z953"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="148.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="148.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1166,33 +1171,33 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -1200,150 +1205,107 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
         <v>48</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
         <v>49</v>
-      </c>
-      <c r="C8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
+        <v>234</v>
+      </c>
+      <c r="B10" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="7"/>
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="7"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="7"/>
-    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A39" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A48" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A49" t="s">
-        <v>108</v>
-      </c>
-      <c r="B49" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="52" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="53" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A53" t="s">
-        <v>112</v>
-      </c>
-      <c r="B53" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="56" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="57" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="58" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="59" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="60" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="63" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -2233,55 +2195,10 @@
     <row r="951" ht="14.25" customHeight="1"/>
     <row r="952" ht="14.25" customHeight="1"/>
     <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{3304E173-E629-4825-B4FA-E24275122099}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2289,16 +2206,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B23"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2335,7 +2252,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2346,7 +2263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -2460,7 +2377,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2473,7 +2390,7 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2481,31 +2398,31 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B21">
-        <v>15</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B22">
         <v>0.1</v>
@@ -2513,20 +2430,65 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C24" t="s">
+        <v>219</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>223</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>225</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>226</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>227</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
@@ -3494,16 +3456,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.26953125" customWidth="1"/>
+    <col min="3" max="3" width="55.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3544,13 +3506,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3578,13 +3540,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -3612,13 +3574,13 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -3646,127 +3608,127 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -3793,691 +3755,741 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" t="s">
         <v>113</v>
       </c>
-      <c r="C15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" t="s">
-        <v>123</v>
-      </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D18" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D21" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F24" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F26" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F27" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F28" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F29" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="F30" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="F31" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C32" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="F32" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B34" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C36" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C38" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C41" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B42" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B43" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
+        <v>169</v>
+      </c>
+      <c r="B44" t="s">
         <v>179</v>
       </c>
-      <c r="B44" t="s">
-        <v>189</v>
-      </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" t="s">
         <v>180</v>
       </c>
-      <c r="B45" t="s">
-        <v>190</v>
-      </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B46" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C46" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" t="s">
+        <v>171</v>
+      </c>
+      <c r="B47" t="s">
         <v>181</v>
       </c>
-      <c r="B47" t="s">
-        <v>191</v>
-      </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
+        <v>172</v>
+      </c>
+      <c r="B48" t="s">
         <v>182</v>
       </c>
-      <c r="B48" t="s">
-        <v>192</v>
-      </c>
       <c r="C48" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" t="s">
+        <v>173</v>
+      </c>
+      <c r="B49" t="s">
         <v>183</v>
       </c>
-      <c r="B49" t="s">
-        <v>193</v>
-      </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" t="s">
+        <v>174</v>
+      </c>
+      <c r="B50" t="s">
         <v>184</v>
       </c>
-      <c r="B50" t="s">
-        <v>194</v>
-      </c>
       <c r="C50" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" t="s">
         <v>185</v>
       </c>
-      <c r="B51" t="s">
-        <v>195</v>
-      </c>
       <c r="C51" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1">
       <c r="A52" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" t="s">
         <v>186</v>
       </c>
-      <c r="B52" t="s">
-        <v>196</v>
-      </c>
       <c r="C52" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
       <c r="A53" t="s">
+        <v>177</v>
+      </c>
+      <c r="B53" t="s">
         <v>187</v>
       </c>
-      <c r="B53" t="s">
-        <v>197</v>
-      </c>
       <c r="C53" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
       <c r="A54" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54" t="s">
         <v>188</v>
       </c>
-      <c r="B54" t="s">
-        <v>198</v>
-      </c>
       <c r="C54" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1">
       <c r="A55" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B55" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B56" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C56" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B57" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C57" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B58" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C58" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B59" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="C59" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1">
       <c r="A60" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C60" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B61" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C61" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B62" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C62" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B63" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C63" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B64" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C64" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B65" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C65" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B66" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C66" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B67" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C67" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="69" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="70" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="71" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="72" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A68" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B68" t="s">
+        <v>220</v>
+      </c>
+      <c r="C68" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A69" t="s">
+        <v>222</v>
+      </c>
+      <c r="B69" t="s">
+        <v>221</v>
+      </c>
+      <c r="C69" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A70" t="s">
+        <v>228</v>
+      </c>
+      <c r="B70" t="s">
+        <v>229</v>
+      </c>
+      <c r="C70" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
+        <v>230</v>
+      </c>
+      <c r="B71" t="s">
+        <v>231</v>
+      </c>
+      <c r="C71" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A72" t="s">
+        <v>232</v>
+      </c>
+      <c r="B72" t="s">
+        <v>233</v>
+      </c>
+      <c r="C72" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="74" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="75" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
updated code for new CR for selecting templates
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Downloads\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1FD63C-2551-4B9E-9733-7C06E1B19DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073978BE-993F-4A27-A4ED-8A279278CC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="289">
   <si>
     <t>Name</t>
   </si>
@@ -894,6 +894,18 @@
   </si>
   <si>
     <t>BotOrchestartorEnvirnoment</t>
+  </si>
+  <si>
+    <t>WorkerSubTypeNotFoundMessage</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_WorkerSubTypeNotFoundMessage</t>
+  </si>
+  <si>
+    <t>WorkerSubTypeNotMatchException</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_WorkerSubTypeNotMatchException</t>
   </si>
 </sst>
 </file>
@@ -3714,8 +3726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -4906,8 +4918,36 @@
         <v>280</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="74" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="73" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A73" t="s">
+        <v>285</v>
+      </c>
+      <c r="B73" t="s">
+        <v>286</v>
+      </c>
+      <c r="C73" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D73" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A74" t="s">
+        <v>287</v>
+      </c>
+      <c r="B74" t="s">
+        <v>288</v>
+      </c>
+      <c r="C74" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D74" t="s">
+        <v>287</v>
+      </c>
+    </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="76" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="77" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Config update with shared asset
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Downloads\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073978BE-993F-4A27-A4ED-8A279278CC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B165122-146A-4A31-8AA1-56C344FE2375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="289">
   <si>
     <t>Name</t>
   </si>
@@ -189,18 +189,12 @@
     <t>Office 365 Tenant ID to access Office 365 Apps using API</t>
   </si>
   <si>
-    <t>P004_SP002_090_BusinessExceptionContacts</t>
-  </si>
-  <si>
     <t>BE_Contacts</t>
   </si>
   <si>
     <t>SE_Contacts</t>
   </si>
   <si>
-    <t>P004_SP002_090_SystemExceptionContacts</t>
-  </si>
-  <si>
     <t>Office 365 App Secret</t>
   </si>
   <si>
@@ -345,15 +339,9 @@
     <t>RuntimeLocalFolderPath</t>
   </si>
   <si>
-    <t>P004_SP002_090_LocalRootFolder</t>
-  </si>
-  <si>
     <t>BE_Contacts_CC</t>
   </si>
   <si>
-    <t>P004_SP002_090_BusinessExceptionCCContacts</t>
-  </si>
-  <si>
     <t>P004_SP002_090_BE_Subject</t>
   </si>
   <si>
@@ -363,9 +351,6 @@
     <t>SE_Contacts_CC</t>
   </si>
   <si>
-    <t>P004_SP002_090_SystemExceptionCCContacts</t>
-  </si>
-  <si>
     <t>P004_SP002_090_SE_Subject</t>
   </si>
   <si>
@@ -384,9 +369,6 @@
     <t>BotMailID</t>
   </si>
   <si>
-    <t>P004_SP002_090_BotMailId</t>
-  </si>
-  <si>
     <t>P004_SP002_090_JRNotFoundException</t>
   </si>
   <si>
@@ -426,9 +408,6 @@
     <t>WorkdayURL</t>
   </si>
   <si>
-    <t>P004_SP002_090_WorkdayURL</t>
-  </si>
-  <si>
     <t>WorkdayLoginException</t>
   </si>
   <si>
@@ -516,15 +495,9 @@
     <t>P004_SP002_090_SummaryTabNotFound</t>
   </si>
   <si>
-    <t>P004_SP002_090_SharepointSiteURL</t>
-  </si>
-  <si>
     <t>P004_SP002_090_SharepointListFilter</t>
   </si>
   <si>
-    <t>P004_SP002_090_SharepointList</t>
-  </si>
-  <si>
     <t>P004_SP002_090_SharepointListColumns</t>
   </si>
   <si>
@@ -552,9 +525,6 @@
     <t>HRDirectorContact</t>
   </si>
   <si>
-    <t>P004_SP002_090_HRDirectorContact</t>
-  </si>
-  <si>
     <t>ListFieldUpdateValue_OfferGenerated</t>
   </si>
   <si>
@@ -586,9 +556,6 @@
   </si>
   <si>
     <t>ListFieldUpdateColumn</t>
-  </si>
-  <si>
-    <t>P004_SP002_090_ListFieldUpdateColumn</t>
   </si>
   <si>
     <t>PersonPeople</t>
@@ -906,6 +873,39 @@
   </si>
   <si>
     <t>P004_SP002_090_WorkerSubTypeNotMatchException</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_EmailAccount</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_WorkdayURL</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SharepointURL</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SharepointListName</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SE_Email</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_BE_Email</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_LocalRootFolder</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SE_EmailCC</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_BE_EmailCC</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_HREmail</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_Status_ColumnDisplayName</t>
   </si>
 </sst>
 </file>
@@ -956,12 +956,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -981,7 +987,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1001,6 +1007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{993BA577-D028-49B5-9D0B-826EDF1209C9}"/>
@@ -1322,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z953"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1370,10 +1377,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -1383,8 +1390,9 @@
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>42</v>
+      <c r="B3" s="2" t="str">
+        <f>Constants!B2</f>
+        <v>DEV</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -1396,7 +1404,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -1404,18 +1412,18 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
         <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
         <v>45</v>
@@ -1426,7 +1434,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
         <v>46</v>
@@ -1438,24 +1446,24 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C10" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2411,7 +2419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2459,7 +2467,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
@@ -2627,136 +2635,136 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B20">
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B21">
         <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B22">
         <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B23">
         <v>0.1</v>
       </c>
       <c r="C23" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B31">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B32">
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -3726,8 +3734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3775,17 +3783,17 @@
     </row>
     <row r="2" spans="1:24" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2" t="str">
         <f>Constants!B2</f>
         <v>DEV</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -3820,7 +3828,7 @@
         <v>DEV</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -3855,7 +3863,7 @@
         <v>DEV</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -3880,152 +3888,152 @@
     </row>
     <row r="5" spans="1:24" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>284</v>
       </c>
       <c r="C5" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
         <v>50</v>
       </c>
+      <c r="B6" s="9" t="s">
+        <v>283</v>
+      </c>
       <c r="C6" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" t="s">
-        <v>104</v>
+        <v>100</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>286</v>
       </c>
       <c r="C7" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>282</v>
       </c>
       <c r="C10" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" t="s">
-        <v>108</v>
+        <v>103</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="C11" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>114</v>
-      </c>
-      <c r="B14" t="s">
-        <v>115</v>
+        <v>109</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>278</v>
       </c>
       <c r="C14" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -4050,902 +4058,902 @@
     </row>
     <row r="15" spans="1:24" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C16" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C18" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C20" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C22" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C23" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C24" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C26" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C27" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C28" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C30" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C31" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C32" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C33" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C34" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C35" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C36" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C37" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>128</v>
-      </c>
-      <c r="B38" t="s">
-        <v>129</v>
+        <v>122</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>279</v>
       </c>
       <c r="C38" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C39" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C40" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C41" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C42" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C43" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B44" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C44" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B45" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C45" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B46" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C46" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C47" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>149</v>
-      </c>
-      <c r="B48" t="s">
-        <v>159</v>
+        <v>142</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>280</v>
       </c>
       <c r="C48" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B49" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C49" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>151</v>
-      </c>
-      <c r="B50" t="s">
-        <v>161</v>
+        <v>144</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>281</v>
       </c>
       <c r="C50" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C51" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C52" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="14.25" customHeight="1">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B53" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C53" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.25" customHeight="1">
       <c r="A54" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C54" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="14.25" customHeight="1">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B55" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C55" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C56" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>170</v>
-      </c>
-      <c r="B57" t="s">
-        <v>171</v>
+        <v>161</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>287</v>
       </c>
       <c r="C57" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B58" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C58" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B59" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C59" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="14.25" customHeight="1">
       <c r="A60" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C60" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B61" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C61" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B62" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C62" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>182</v>
-      </c>
-      <c r="B63" t="s">
-        <v>183</v>
+        <v>172</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>288</v>
       </c>
       <c r="C63" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B64" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C64" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B65" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C65" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B66" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C66" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="14.25" customHeight="1">
       <c r="A67" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B67" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C67" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="14.25" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B68" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="C68" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="14.25" customHeight="1">
       <c r="A69" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B69" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C69" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="14.25" customHeight="1">
       <c r="A70" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B70" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C70" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="14.25" customHeight="1">
       <c r="A71" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B71" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C71" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="14.25" customHeight="1">
       <c r="A72" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B72" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C72" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="14.25" customHeight="1">
       <c r="A73" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="B73" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="C73" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D73" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="14.25" customHeight="1">
       <c r="A74" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="B74" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="C74" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D74" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added building name and address to queue
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Downloads\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B165122-146A-4A31-8AA1-56C344FE2375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA901EF-AC6A-4ED5-AC71-D3D443CD1676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="296">
   <si>
     <t>Name</t>
   </si>
@@ -906,6 +906,27 @@
   </si>
   <si>
     <t>P004_Shared_090_Status_ColumnDisplayName</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BuildingName_Address</t>
+  </si>
+  <si>
+    <t>BuildingName_Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BuildingName - Address | BuildingName - Address </t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BuildingName_NotFoundMsg</t>
+  </si>
+  <si>
+    <t>BuildingName_NotFoundMsg</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BuildingAddress_NotFoundMsg</t>
+  </si>
+  <si>
+    <t>BuildingAddress_NotFoundMsg</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z953"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3734,8 +3755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -4956,9 +4977,51 @@
         <v>276</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="76" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="77" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A75" t="s">
+        <v>290</v>
+      </c>
+      <c r="B75" t="s">
+        <v>289</v>
+      </c>
+      <c r="C75" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D75" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A76" t="s">
+        <v>293</v>
+      </c>
+      <c r="B76" t="s">
+        <v>292</v>
+      </c>
+      <c r="C76" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D76" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A77" t="s">
+        <v>295</v>
+      </c>
+      <c r="B77" t="s">
+        <v>294</v>
+      </c>
+      <c r="C77" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D77" t="s">
+        <v>295</v>
+      </c>
+    </row>
     <row r="78" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="79" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="80" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Update Templates for Building name and address
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Downloads\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA901EF-AC6A-4ED5-AC71-D3D443CD1676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD711ED-DD8F-4D88-8716-BF3A0A398FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="298">
   <si>
     <t>Name</t>
   </si>
@@ -927,6 +927,12 @@
   </si>
   <si>
     <t>BuildingAddress_NotFoundMsg</t>
+  </si>
+  <si>
+    <t>BuildingNameToReplace</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BuildingNameToReplace</t>
   </si>
 </sst>
 </file>
@@ -977,7 +983,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -987,6 +993,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1008,7 +1020,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1029,6 +1041,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{993BA577-D028-49B5-9D0B-826EDF1209C9}"/>
@@ -3756,7 +3769,7 @@
   <dimension ref="A1:X999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -4978,7 +4991,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A75" t="s">
+      <c r="A75" s="10" t="s">
         <v>290</v>
       </c>
       <c r="B75" t="s">
@@ -4993,7 +5006,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A76" t="s">
+      <c r="A76" s="10" t="s">
         <v>293</v>
       </c>
       <c r="B76" t="s">
@@ -5008,7 +5021,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A77" t="s">
+      <c r="A77" s="10" t="s">
         <v>295</v>
       </c>
       <c r="B77" t="s">
@@ -5022,7 +5035,21 @@
         <v>295</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A78" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C78" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D78" t="s">
+        <v>296</v>
+      </c>
+    </row>
     <row r="79" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="80" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="81" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
updated code after CR for building name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Downloads\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56174C\Downloads\Bot Code Folder\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD711ED-DD8F-4D88-8716-BF3A0A398FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23EFD8A-2D20-4C06-AC9A-F4143327E86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1065,9 +1065,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1105,7 +1105,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1211,7 +1211,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1353,7 +1353,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2453,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2683,7 +2683,7 @@
         <v>126</v>
       </c>
       <c r="B20">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
         <v>126</v>
@@ -2694,7 +2694,7 @@
         <v>127</v>
       </c>
       <c r="B21">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
         <v>127</v>
@@ -2705,7 +2705,7 @@
         <v>128</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="C22" t="s">
         <v>128</v>
@@ -3768,7 +3768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Config for PROD folder
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56174C\Downloads\Bot Code Folder\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23EFD8A-2D20-4C06-AC9A-F4143327E86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AEA8E4-8BAB-4D10-BD43-8CE4ACE88490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>Office365_AppID</t>
   </si>
   <si>
@@ -933,6 +930,9 @@
   </si>
   <si>
     <t>P004_SP002_090_BuildingNameToReplace</t>
+  </si>
+  <si>
+    <t>PROD</t>
   </si>
 </sst>
 </file>
@@ -1363,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z953"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1411,10 +1411,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B3" s="2" t="str">
         <f>Constants!B2</f>
-        <v>DEV</v>
+        <v>PROD</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -1438,7 +1438,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -1446,58 +1446,58 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" t="s">
         <v>200</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>201</v>
-      </c>
-      <c r="C10" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2453,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2501,10 +2501,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>297</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2669,136 +2669,136 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20">
         <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B21">
         <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B22">
         <v>150</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23">
         <v>0.1</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" t="s">
         <v>184</v>
-      </c>
-      <c r="C25" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B31">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B32">
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -3768,7 +3768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A59" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
@@ -3817,17 +3817,17 @@
     </row>
     <row r="2" spans="1:24" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
         <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
       </c>
       <c r="C2" t="str">
         <f>Constants!B2</f>
-        <v>DEV</v>
+        <v>PROD</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -3852,17 +3852,17 @@
     </row>
     <row r="3" spans="1:24" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="str">
         <f>Constants!B2</f>
-        <v>DEV</v>
+        <v>PROD</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -3887,17 +3887,17 @@
     </row>
     <row r="4" spans="1:24" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="str">
         <f>Constants!B2</f>
-        <v>DEV</v>
+        <v>PROD</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -3922,152 +3922,152 @@
     </row>
     <row r="5" spans="1:24" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C10" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C14" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -4092,962 +4092,962 @@
     </row>
     <row r="15" spans="1:24" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C30" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C32" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C33" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1">
       <c r="A34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" t="s">
         <v>114</v>
       </c>
-      <c r="B34" t="s">
-        <v>115</v>
-      </c>
       <c r="C34" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C35" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14.25" customHeight="1">
       <c r="A37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" t="s">
         <v>120</v>
       </c>
-      <c r="B37" t="s">
-        <v>121</v>
-      </c>
       <c r="C37" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C38" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14.25" customHeight="1">
       <c r="A39" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" t="s">
         <v>123</v>
       </c>
-      <c r="B39" t="s">
-        <v>124</v>
-      </c>
       <c r="C39" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.25" customHeight="1">
       <c r="A40" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" t="s">
         <v>131</v>
       </c>
-      <c r="B40" t="s">
-        <v>132</v>
-      </c>
       <c r="C40" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="14.25" customHeight="1">
       <c r="A41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" t="s">
         <v>133</v>
       </c>
-      <c r="B41" t="s">
-        <v>134</v>
-      </c>
       <c r="C41" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C43" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C44" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C45" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="14.25" customHeight="1">
       <c r="A46" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" t="s">
         <v>173</v>
       </c>
-      <c r="B46" t="s">
-        <v>174</v>
-      </c>
       <c r="C46" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C47" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C48" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C49" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C50" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C51" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C52" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="14.25" customHeight="1">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C53" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.25" customHeight="1">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C54" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="14.25" customHeight="1">
       <c r="A55" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55" t="s">
         <v>157</v>
       </c>
-      <c r="B55" t="s">
-        <v>158</v>
-      </c>
       <c r="C55" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C56" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C57" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.25" customHeight="1">
       <c r="A58" t="s">
+        <v>161</v>
+      </c>
+      <c r="B58" t="s">
         <v>162</v>
       </c>
-      <c r="B58" t="s">
-        <v>163</v>
-      </c>
       <c r="C58" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="14.25" customHeight="1">
       <c r="A59" t="s">
+        <v>163</v>
+      </c>
+      <c r="B59" t="s">
         <v>164</v>
       </c>
-      <c r="B59" t="s">
-        <v>165</v>
-      </c>
       <c r="C59" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="14.25" customHeight="1">
       <c r="A60" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B60" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C60" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="14.25" customHeight="1">
       <c r="A61" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" t="s">
         <v>168</v>
       </c>
-      <c r="B61" t="s">
-        <v>169</v>
-      </c>
       <c r="C61" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14.25" customHeight="1">
       <c r="A62" t="s">
+        <v>169</v>
+      </c>
+      <c r="B62" t="s">
         <v>170</v>
       </c>
-      <c r="B62" t="s">
-        <v>171</v>
-      </c>
       <c r="C62" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C63" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.25" customHeight="1">
       <c r="A64" t="s">
+        <v>174</v>
+      </c>
+      <c r="B64" t="s">
         <v>175</v>
       </c>
-      <c r="B64" t="s">
-        <v>176</v>
-      </c>
       <c r="C64" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B65" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C65" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B66" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C66" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="14.25" customHeight="1">
       <c r="A67" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" t="s">
         <v>181</v>
       </c>
-      <c r="B67" t="s">
-        <v>182</v>
-      </c>
       <c r="C67" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="14.25" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B68" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C68" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="14.25" customHeight="1">
       <c r="A69" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B69" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C69" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="14.25" customHeight="1">
       <c r="A70" t="s">
+        <v>193</v>
+      </c>
+      <c r="B70" t="s">
         <v>194</v>
       </c>
-      <c r="B70" t="s">
-        <v>195</v>
-      </c>
       <c r="C70" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="14.25" customHeight="1">
       <c r="A71" t="s">
+        <v>195</v>
+      </c>
+      <c r="B71" t="s">
         <v>196</v>
       </c>
-      <c r="B71" t="s">
-        <v>197</v>
-      </c>
       <c r="C71" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="14.25" customHeight="1">
       <c r="A72" t="s">
+        <v>197</v>
+      </c>
+      <c r="B72" t="s">
         <v>198</v>
       </c>
-      <c r="B72" t="s">
-        <v>199</v>
-      </c>
       <c r="C72" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="14.25" customHeight="1">
       <c r="A73" t="s">
+        <v>273</v>
+      </c>
+      <c r="B73" t="s">
         <v>274</v>
       </c>
-      <c r="B73" t="s">
-        <v>275</v>
-      </c>
       <c r="C73" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D73" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="14.25" customHeight="1">
       <c r="A74" t="s">
+        <v>275</v>
+      </c>
+      <c r="B74" t="s">
         <v>276</v>
       </c>
-      <c r="B74" t="s">
-        <v>277</v>
-      </c>
       <c r="C74" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D74" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1">
       <c r="A75" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B75" t="s">
+        <v>288</v>
+      </c>
+      <c r="C75" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D75" t="s">
         <v>290</v>
-      </c>
-      <c r="B75" t="s">
-        <v>289</v>
-      </c>
-      <c r="C75" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
-      </c>
-      <c r="D75" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="14.25" customHeight="1">
       <c r="A76" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B76" t="s">
+        <v>291</v>
+      </c>
+      <c r="C76" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D76" t="s">
         <v>292</v>
-      </c>
-      <c r="C76" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
-      </c>
-      <c r="D76" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="14.25" customHeight="1">
       <c r="A77" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B77" t="s">
+        <v>293</v>
+      </c>
+      <c r="C77" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D77" t="s">
         <v>294</v>
-      </c>
-      <c r="C77" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
-      </c>
-      <c r="D77" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="14.25" customHeight="1">
       <c r="A78" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B78" t="s">
         <v>296</v>
       </c>
-      <c r="B78" t="s">
-        <v>297</v>
-      </c>
       <c r="C78" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D78" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
update for Prod Sharepoint to download Templates
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56174C\Downloads\Bot Code Folder\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76963E4A-E102-427A-B41D-14DD84BBD8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3160178-B4DE-4D93-8397-B343BDCC8064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="301">
   <si>
     <t>Name</t>
   </si>
@@ -930,6 +930,15 @@
   </si>
   <si>
     <t>P004_SP002_090_BuildingNameToReplace</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_BOT_SharepointURL</t>
+  </si>
+  <si>
+    <t>BOT_SharepointURL</t>
+  </si>
+  <si>
+    <t>BOT_SharepointURL where stores templates files</t>
   </si>
   <si>
     <t>PROD</t>
@@ -1065,9 +1074,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1105,7 +1114,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1211,7 +1220,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1353,7 +1362,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1363,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z953"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2453,8 +2462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2504,7 +2513,7 @@
         <v>272</v>
       </c>
       <c r="B2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3768,8 +3777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -5050,7 +5059,21 @@
         <v>295</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A79" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B79" t="s">
+        <v>297</v>
+      </c>
+      <c r="C79" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>PROD/P004_NewHireCommunication</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
     <row r="80" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="81" ht="14.25" customHeight="1"/>
     <row r="82" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added updated Workday lib for login with userid case
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56174C\Downloads\Bot Code Folder\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3160178-B4DE-4D93-8397-B343BDCC8064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C785445-7DFE-4782-BF7E-4F485D8B088B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="304">
   <si>
     <t>Name</t>
   </si>
@@ -941,7 +941,16 @@
     <t>BOT_SharepointURL where stores templates files</t>
   </si>
   <si>
+    <t>WorkdayLoginCredentialAsset</t>
+  </si>
+  <si>
+    <t>WorkdayLoginCredentialAssetQrchestratorFolder</t>
+  </si>
+  <si>
     <t>PROD</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_WorkdayLoginCredentialAsset</t>
   </si>
 </sst>
 </file>
@@ -1372,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z953"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1509,8 +1518,29 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B12" t="s">
+        <v>303</v>
+      </c>
+      <c r="C12" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="C13" t="s">
+        <v>301</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2463,7 +2493,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2513,7 +2543,7 @@
         <v>272</v>
       </c>
       <c r="B2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2681,7 +2711,7 @@
         <v>124</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>124</v>
@@ -3777,8 +3807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
1-Added sharepoint name search in workday. 2-Added Salary formatting. 3-Moved constant sheet config values to assets sheet for Adding queue information to postpone item for Signed offer letter.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56174C\Downloads\Bot Code Folder\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56174C\Downloads\PROD\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C785445-7DFE-4782-BF7E-4F485D8B088B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5DA757-BE23-456D-9D99-B6BC69A8B303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="309">
   <si>
     <t>Name</t>
   </si>
@@ -947,10 +947,25 @@
     <t>WorkdayLoginCredentialAssetQrchestratorFolder</t>
   </si>
   <si>
+    <t>P004_SP002_090_WorkdayLoginCredentialAsset</t>
+  </si>
+  <si>
     <t>PROD</t>
   </si>
   <si>
-    <t>P004_SP002_090_WorkdayLoginCredentialAsset</t>
+    <t>P004_SP002_090_DaysToAddForMonday</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_DaysToAddForTuesday</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_DaysToAddForWednesday</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_DaysToAddForThrusday</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_DaysToAddForFriday</t>
   </si>
 </sst>
 </file>
@@ -1381,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z953"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1523,7 +1538,7 @@
         <v>300</v>
       </c>
       <c r="B12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C12" t="s">
         <v>300</v>
@@ -2490,10 +2505,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z989"/>
+  <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2542,8 +2557,8 @@
       <c r="A2" t="s">
         <v>272</v>
       </c>
-      <c r="B2" t="s">
-        <v>302</v>
+      <c r="B2" s="9" t="s">
+        <v>303</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2785,61 +2800,11 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
-        <v>188</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" t="s">
-        <v>189</v>
-      </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" t="s">
-        <v>190</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
-        <v>191</v>
-      </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>192</v>
-      </c>
-      <c r="B32">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
-        <v>207</v>
-      </c>
-    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -3792,11 +3757,6 @@
     <row r="982" ht="14.25" customHeight="1"/>
     <row r="983" ht="14.25" customHeight="1"/>
     <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3807,8 +3767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -5104,23 +5064,93 @@
         <v>299</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="80" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A80" t="s">
+        <v>188</v>
+      </c>
+      <c r="B80" t="s">
+        <v>304</v>
+      </c>
+      <c r="C80" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D80" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A81" t="s">
+        <v>189</v>
+      </c>
+      <c r="B81" t="s">
+        <v>305</v>
+      </c>
+      <c r="C81" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D81" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A82" t="s">
+        <v>190</v>
+      </c>
+      <c r="B82" t="s">
+        <v>306</v>
+      </c>
+      <c r="C82" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D82" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A83" t="s">
+        <v>191</v>
+      </c>
+      <c r="B83" t="s">
+        <v>307</v>
+      </c>
+      <c r="C83" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D83" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A84" t="s">
+        <v>192</v>
+      </c>
+      <c r="B84" t="s">
+        <v>308</v>
+      </c>
+      <c r="C84" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D84" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="86" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="87" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="88" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="89" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="90" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="91" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="92" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="93" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="94" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="95" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="96" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="97" ht="14.25" customHeight="1"/>
     <row r="98" ht="14.25" customHeight="1"/>
     <row r="99" ht="14.25" customHeight="1"/>

</xml_diff>